<commit_message>
change in file name
</commit_message>
<xml_diff>
--- a/data/D_infections_volatility_tracker.xlsx
+++ b/data/D_infections_volatility_tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nezasmid/Desktop/VU-MSc/RP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nezasmid/research-project-bitcoin-prices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3DC3D4E-24CA-604D-A275-30AEF08630CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625809E8-7905-2247-97E7-0E312C53135C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D1ADA8B5-343A-EA4B-B680-17D2B20F255A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{D1ADA8B5-343A-EA4B-B680-17D2B20F255A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>All_Infectious_EMV_Data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>day</t>
   </si>
@@ -429,9 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9D9267-0150-0846-B40E-CF7E9E2C0512}">
   <dimension ref="A1:E751"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A735" workbookViewId="0">
-      <selection activeCell="G764" sqref="G764"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -439,25 +434,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>